<commit_message>
update link to codebook + about_elan
</commit_message>
<xml_diff>
--- a/themes/elancholia/visual_generators/elan_classification.xlsx
+++ b/themes/elancholia/visual_generators/elan_classification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\juju\lumc\information-products\other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ldeschipper\juju\elan-dcc.github.io\themes\elancholia\visual_generators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C923FF-BD60-4F3A-9D12-083709FB3E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55FA5564-5742-4B28-9B09-4DA02EFF6B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12870" yWindow="465" windowWidth="13800" windowHeight="15135" xr2:uid="{5B043674-7E8B-4440-9A4D-67744926348C}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{5B043674-7E8B-4440-9A4D-67744926348C}"/>
   </bookViews>
   <sheets>
     <sheet name="classification" sheetId="1" r:id="rId1"/>
@@ -598,7 +598,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>